<commit_message>
Update reference result after changes for compressed files.  Add OGRVectorFormats.
</commit_message>
<xml_diff>
--- a/Notes/OGRVectorFormats.xlsx
+++ b/Notes/OGRVectorFormats.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Projects\TauDEM\Programming\TauDEM5GDAL\Notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dtarb\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="6630"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6705"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$1:$E$90</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$1:$F$90</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="197">
   <si>
     <t>OGR Vector Formats</t>
   </si>
@@ -614,7 +614,10 @@
     <t>Don’t have examples</t>
   </si>
   <si>
-    <t>Try this</t>
+    <t>Not for persistent disk storage</t>
+  </si>
+  <si>
+    <t>We can try this</t>
   </si>
 </sst>
 </file>
@@ -991,7 +994,7 @@
   <dimension ref="A1:G90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1284,7 +1287,7 @@
         <v>9</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -1486,7 +1489,7 @@
       <c r="E26" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G26" s="7" t="s">
+      <c r="G26" s="8" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1526,7 +1529,9 @@
       <c r="E28" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G28" s="8"/>
+      <c r="G28" s="8" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
@@ -1585,7 +1590,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>58</v>
       </c>
@@ -1645,7 +1650,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>63</v>
       </c>
@@ -1682,7 +1687,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>65</v>
       </c>
@@ -1702,7 +1707,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>66</v>
       </c>
@@ -1870,7 +1875,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>82</v>
       </c>
@@ -1890,7 +1895,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>84</v>
       </c>
@@ -1910,7 +1915,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>85</v>
       </c>
@@ -1930,7 +1935,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>86</v>
       </c>
@@ -1947,7 +1952,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>88</v>
       </c>
@@ -1964,7 +1969,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>90</v>
       </c>
@@ -1984,7 +1989,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>92</v>
       </c>
@@ -2000,8 +2005,11 @@
       <c r="E53" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G53" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>93</v>
       </c>
@@ -2021,7 +2029,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>94</v>
       </c>
@@ -2041,7 +2049,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>95</v>
       </c>
@@ -2061,7 +2069,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>97</v>
       </c>
@@ -2081,7 +2089,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>99</v>
       </c>
@@ -2101,7 +2109,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>100</v>
       </c>
@@ -2121,7 +2129,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>102</v>
       </c>
@@ -2141,7 +2149,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>104</v>
       </c>
@@ -2161,7 +2169,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>106</v>
       </c>
@@ -2178,7 +2186,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>43</v>
       </c>
@@ -2195,7 +2203,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>108</v>
       </c>
@@ -2235,7 +2243,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
         <v>112</v>
       </c>
@@ -2694,7 +2702,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C1:E90">
+  <autoFilter ref="C1:F90">
     <filterColumn colId="0">
       <filters blank="1">
         <filter val="Creation"/>
@@ -2705,6 +2713,11 @@
       <filters blank="1">
         <filter val="Compiled by default"/>
         <filter val="Yes"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="3">
+      <filters blank="1">
+        <filter val="using internal PCIDSK SDK (from GDAL 1.7.0)"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Update OGRVectorFormats.xlsx Notes spreadsheet
</commit_message>
<xml_diff>
--- a/Notes/OGRVectorFormats.xlsx
+++ b/Notes/OGRVectorFormats.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dtarb\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Projects\TauDEM\Programming\TauDEM5GDAL\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="196">
   <si>
     <t>OGR Vector Formats</t>
   </si>
@@ -593,12 +593,6 @@
     <t xml:space="preserve"> (read supports need libpoppler or libpodofo support)</t>
   </si>
   <si>
-    <t>See if we can get FileGDB API.  May require Arc License</t>
-  </si>
-  <si>
-    <t>See if we can do this using  ODBC from Excel</t>
-  </si>
-  <si>
     <t>Explore this</t>
   </si>
   <si>
@@ -618,12 +612,15 @@
   </si>
   <si>
     <t>We can try this</t>
+  </si>
+  <si>
+    <t>Are we using this one?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -990,11 +987,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:G90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <pane ySplit="3" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1016,10 +1013,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -1045,7 +1042,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -1062,10 +1059,10 @@
         <v>9</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
@@ -1085,7 +1082,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
@@ -1105,7 +1102,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>14</v>
       </c>
@@ -1122,7 +1119,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>16</v>
       </c>
@@ -1139,7 +1136,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>18</v>
       </c>
@@ -1173,10 +1170,10 @@
         <v>9</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>22</v>
       </c>
@@ -1210,7 +1207,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>26</v>
       </c>
@@ -1230,7 +1227,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>27</v>
       </c>
@@ -1250,7 +1247,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>29</v>
       </c>
@@ -1287,10 +1284,10 @@
         <v>9</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>33</v>
       </c>
@@ -1310,7 +1307,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>35</v>
       </c>
@@ -1330,7 +1327,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>37</v>
       </c>
@@ -1350,7 +1347,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>39</v>
       </c>
@@ -1370,7 +1367,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>41</v>
       </c>
@@ -1387,7 +1384,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>42</v>
       </c>
@@ -1407,7 +1404,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>43</v>
       </c>
@@ -1426,11 +1423,9 @@
       <c r="F23" t="s">
         <v>163</v>
       </c>
-      <c r="G23" s="7" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G23" s="8"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>45</v>
       </c>
@@ -1449,11 +1444,9 @@
       <c r="F24" t="s">
         <v>161</v>
       </c>
-      <c r="G24" s="7" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G24" s="8"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>47</v>
       </c>
@@ -1489,11 +1482,11 @@
       <c r="E26" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G26" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G26" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>50</v>
       </c>
@@ -1529,8 +1522,8 @@
       <c r="E28" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G28" s="8" t="s">
-        <v>196</v>
+      <c r="G28" s="7" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1550,7 +1543,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>54</v>
       </c>
@@ -1570,7 +1563,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>56</v>
       </c>
@@ -1590,7 +1583,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>58</v>
       </c>
@@ -1610,7 +1603,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>59</v>
       </c>
@@ -1630,7 +1623,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>61</v>
       </c>
@@ -1650,7 +1643,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>63</v>
       </c>
@@ -1687,7 +1680,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>65</v>
       </c>
@@ -1707,7 +1700,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>66</v>
       </c>
@@ -1727,7 +1720,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>67</v>
       </c>
@@ -1764,7 +1757,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>71</v>
       </c>
@@ -1781,7 +1774,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>73</v>
       </c>
@@ -1798,7 +1791,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>75</v>
       </c>
@@ -1818,7 +1811,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>77</v>
       </c>
@@ -1835,7 +1828,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>79</v>
       </c>
@@ -1855,7 +1848,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>81</v>
       </c>
@@ -1875,7 +1868,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>82</v>
       </c>
@@ -1895,7 +1888,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>84</v>
       </c>
@@ -1915,7 +1908,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>85</v>
       </c>
@@ -1969,7 +1962,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>90</v>
       </c>
@@ -2006,10 +1999,10 @@
         <v>9</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>93</v>
       </c>
@@ -2029,7 +2022,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>94</v>
       </c>
@@ -2049,7 +2042,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>95</v>
       </c>
@@ -2069,7 +2062,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>97</v>
       </c>
@@ -2089,7 +2082,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>99</v>
       </c>
@@ -2109,7 +2102,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="59" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>100</v>
       </c>
@@ -2129,7 +2122,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="60" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>102</v>
       </c>
@@ -2149,7 +2142,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>104</v>
       </c>
@@ -2169,7 +2162,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>106</v>
       </c>
@@ -2186,7 +2179,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>43</v>
       </c>
@@ -2202,8 +2195,11 @@
       <c r="E63" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G63" s="7" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>108</v>
       </c>
@@ -2243,7 +2239,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
         <v>112</v>
       </c>
@@ -2263,7 +2259,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
         <v>114</v>
       </c>
@@ -2280,7 +2276,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>115</v>
       </c>
@@ -2317,7 +2313,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
         <v>119</v>
       </c>
@@ -2337,7 +2333,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="71" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>120</v>
       </c>
@@ -2354,7 +2350,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
         <v>122</v>
       </c>
@@ -2371,7 +2367,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
         <v>124</v>
       </c>
@@ -2388,7 +2384,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
         <v>125</v>
       </c>
@@ -2405,7 +2401,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="75" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
         <v>127</v>
       </c>
@@ -2439,7 +2435,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="77" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
         <v>132</v>
       </c>
@@ -2459,7 +2455,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
         <v>134</v>
       </c>
@@ -2479,10 +2475,10 @@
         <v>181</v>
       </c>
       <c r="G78" s="7" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
         <v>136</v>
       </c>
@@ -2499,7 +2495,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="80" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
         <v>137</v>
       </c>
@@ -2519,7 +2515,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
         <v>138</v>
       </c>
@@ -2536,7 +2532,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="82" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
         <v>140</v>
       </c>
@@ -2553,7 +2549,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="83" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>142</v>
       </c>
@@ -2570,7 +2566,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>144</v>
       </c>
@@ -2587,7 +2583,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>146</v>
       </c>
@@ -2607,7 +2603,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="86" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
         <v>148</v>
       </c>
@@ -2627,7 +2623,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="87" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
         <v>150</v>
       </c>
@@ -2647,7 +2643,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="88" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
         <v>152</v>
       </c>
@@ -2664,7 +2660,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="89" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
         <v>154</v>
       </c>
@@ -2702,25 +2698,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C1:F90">
-    <filterColumn colId="0">
-      <filters blank="1">
-        <filter val="Creation"/>
-        <filter val="Yes"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="2">
-      <filters blank="1">
-        <filter val="Compiled by default"/>
-        <filter val="Yes"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="3">
-      <filters blank="1">
-        <filter val="using internal PCIDSK SDK (from GDAL 1.7.0)"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="C1:F90"/>
   <hyperlinks>
     <hyperlink ref="A4" r:id="rId1" display="http://www.gdal.org/drv_aeronavfaa.html"/>
     <hyperlink ref="A5" r:id="rId2" display="http://www.gdal.org/drv_amigocloud.html"/>

</xml_diff>